<commit_message>
added developer comments for login faeture
</commit_message>
<xml_diff>
--- a/Code Testing.xlsx
+++ b/Code Testing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aditya\Desktop\Tech is all you need\Enterprise-Level-Chatbot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D871E1A6-C679-4818-B073-D886E76997E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1835C613-BA0A-49B1-8F70-B43C66264750}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
   <si>
     <t>Tracking Commit</t>
   </si>
@@ -98,13 +98,25 @@
   </si>
   <si>
     <t>left</t>
+  </si>
+  <si>
+    <t>Not sure, we will have to monitor this since there seems that is missing since sometimes the browser doesn't keeps the session_token with itself when the server dies(right know it is doing)</t>
+  </si>
+  <si>
+    <t>Developer comments-</t>
+  </si>
+  <si>
+    <t>The developer closed server and  restrated the pc still can the cookie in the brower tools(even now u can see the server is close but still can c the cookie)</t>
+  </si>
+  <si>
+    <t>This is the token expiry time(which is correct this the token will stay)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,8 +159,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -158,6 +178,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -175,13 +201,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -200,6 +232,99 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1069362</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>172891</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>305951</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>49485</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF9968BE-FA9A-4410-9165-B9D45C3C6AF3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1069362" y="3854824"/>
+          <a:ext cx="6171429" cy="4333333"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>973311</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>527983</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>157194</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED76259A-62DC-5D2E-69F8-22BB96326831}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7908151" y="4239026"/>
+          <a:ext cx="4914286" cy="714286"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -465,10 +590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="119" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -476,7 +601,7 @@
     <col min="1" max="1" width="42.5546875" customWidth="1"/>
     <col min="3" max="3" width="49.6640625" customWidth="1"/>
     <col min="4" max="4" width="15.21875" customWidth="1"/>
-    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="5" max="5" width="27.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -572,8 +697,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+    <row r="8" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
         <v>19</v>
       </c>
       <c r="B8">
@@ -585,8 +710,21 @@
       <c r="D8" t="s">
         <v>13</v>
       </c>
-      <c r="E8" t="s">
-        <v>22</v>
+      <c r="E8" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E12" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -595,6 +733,7 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">

</xml_diff>